<commit_message>
Document how to compare with historical PHE data
</commit_message>
<xml_diff>
--- a/data/raw/Historic COVID-19 Dashboard Data.xlsx
+++ b/data/raw/Historic COVID-19 Dashboard Data.xlsx
@@ -20,10 +20,6 @@
     <sheet name="UTLAs" sheetId="3" r:id="rId6"/>
     <sheet name="Recovered patients" sheetId="6" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">UTLAs!$A$8:$AD$159</definedName>
   </definedNames>
@@ -1322,15 +1318,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1360,74 +1356,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ReadMe"/>
-      <sheetName val="Countries"/>
-      <sheetName val="UTLA"/>
-      <sheetName val="NHSRegions"/>
-      <sheetName val="PCons"/>
-      <sheetName val="DailyConfirmedCases UK"/>
-      <sheetName val="SummaryStats"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1">
-        <row r="2">
-          <cell r="C2">
-            <v>39814</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ReadMe"/>
-      <sheetName val="Countries"/>
-      <sheetName val="UTLA"/>
-      <sheetName val="NHSRegions"/>
-      <sheetName val="PCons"/>
-      <sheetName val="DailyConfirmedCases UK"/>
-      <sheetName val="SummaryStats"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
-        <row r="2">
-          <cell r="H2">
-            <v>3345</v>
-          </cell>
-          <cell r="J2">
-            <v>2853</v>
-          </cell>
-          <cell r="L2">
-            <v>998</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1780,7 +1708,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
@@ -2576,11 +2504,33 @@
       <c r="A76" s="23">
         <v>43927</v>
       </c>
-      <c r="B76" s="34">
+      <c r="B76" s="33">
         <v>3802</v>
       </c>
-      <c r="C76" s="34">
+      <c r="C76" s="33">
         <v>51608</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="23">
+        <v>43928</v>
+      </c>
+      <c r="B77" s="33">
+        <v>3634</v>
+      </c>
+      <c r="C77" s="33">
+        <v>55242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="23">
+        <v>43929</v>
+      </c>
+      <c r="B78" s="33">
+        <v>5491</v>
+      </c>
+      <c r="C78" s="33">
+        <v>60733</v>
       </c>
     </row>
   </sheetData>
@@ -2590,7 +2540,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -3157,28 +3107,74 @@
       <c r="A36" s="16">
         <v>43927</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B36" s="34">
         <v>439</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="34">
         <v>5373</v>
       </c>
-      <c r="D36" s="35">
+      <c r="D36" s="34">
         <v>4897</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="34">
         <v>220</v>
       </c>
-      <c r="F36" s="35">
+      <c r="F36" s="34">
         <v>193</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G36" s="34">
         <v>63</v>
       </c>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="32"/>
+      <c r="A37" s="16">
+        <v>43928</v>
+      </c>
+      <c r="B37" s="34">
+        <v>786</v>
+      </c>
+      <c r="C37" s="34">
+        <v>6159</v>
+      </c>
+      <c r="D37" s="34">
+        <v>5655</v>
+      </c>
+      <c r="E37" s="34">
+        <v>222</v>
+      </c>
+      <c r="F37" s="34">
+        <v>212</v>
+      </c>
+      <c r="G37" s="34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
+        <v>43929</v>
+      </c>
+      <c r="B38" s="34">
+        <v>938</v>
+      </c>
+      <c r="C38" s="34">
+        <v>7097</v>
+      </c>
+      <c r="D38" s="34">
+        <v>6483</v>
+      </c>
+      <c r="E38" s="34">
+        <v>296</v>
+      </c>
+      <c r="F38" s="34">
+        <v>245</v>
+      </c>
+      <c r="G38" s="34">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3190,7 +3186,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AG13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -3208,46 +3204,47 @@
     <col min="21" max="21" width="10.7109375" customWidth="1"/>
     <col min="22" max="24" width="10.7109375" style="21" customWidth="1"/>
     <col min="25" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>326</v>
       </c>
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B6" s="11"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3341,8 +3338,14 @@
       <c r="AE8" s="3">
         <v>43927</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF8" s="3">
+        <v>43928</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>43929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -3431,14 +3434,19 @@
         <v>34707</v>
       </c>
       <c r="AD9" s="26">
-        <f>[1]Countries!$C$2</f>
         <v>39814</v>
       </c>
       <c r="AE9" s="26">
         <v>42990</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF9" s="26">
+        <v>45968</v>
+      </c>
+      <c r="AG9" s="26">
+        <v>50756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
@@ -3522,17 +3530,22 @@
         <v>3001</v>
       </c>
       <c r="AC10" s="8">
-        <f>[2]SummaryStats!$H$2</f>
         <v>3345</v>
       </c>
-      <c r="AD10" s="33">
+      <c r="AD10" s="32">
         <v>3706</v>
       </c>
-      <c r="AE10" s="33">
+      <c r="AE10" s="32">
         <v>3961</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF10" s="32">
+        <v>4229</v>
+      </c>
+      <c r="AG10" s="32">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -3616,17 +3629,22 @@
         <v>2466</v>
       </c>
       <c r="AC11" s="8">
-        <f>[2]SummaryStats!$J$2</f>
         <v>2853</v>
       </c>
-      <c r="AD11" s="33">
+      <c r="AD11" s="32">
         <v>3197</v>
       </c>
-      <c r="AE11" s="33">
+      <c r="AE11" s="32">
         <v>3499</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF11" s="32">
+        <v>3790</v>
+      </c>
+      <c r="AG11" s="32">
+        <v>4073</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
@@ -3710,17 +3728,22 @@
         <v>904</v>
       </c>
       <c r="AC12" s="8">
-        <f>[2]SummaryStats!$L$2</f>
         <v>998</v>
       </c>
-      <c r="AD12" s="33">
+      <c r="AD12" s="32">
         <v>1089</v>
       </c>
-      <c r="AE12" s="33">
+      <c r="AE12" s="32">
         <v>1158</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF12" s="32">
+        <v>1255</v>
+      </c>
+      <c r="AG12" s="32">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -3809,6 +3832,12 @@
       </c>
       <c r="AE13" s="4">
         <v>51608</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>55242</v>
+      </c>
+      <c r="AG13" s="4">
+        <v>60733</v>
       </c>
     </row>
   </sheetData>
@@ -3822,7 +3851,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -3838,42 +3867,42 @@
     <col min="22" max="24" width="10.7109375" style="21" customWidth="1"/>
     <col min="25" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="30" width="10.7109375" style="21" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B6" s="11"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -3897,7 +3926,7 @@
       <c r="Z7" s="21"/>
       <c r="AA7" s="21"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3991,8 +4020,14 @@
       <c r="AE8" s="3">
         <v>43927</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF8" s="3">
+        <v>43928</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>43929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -4084,8 +4119,14 @@
       <c r="AE9" s="6">
         <v>1723</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF9" s="6">
+        <v>1818</v>
+      </c>
+      <c r="AG9" s="6">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -4179,8 +4220,14 @@
       <c r="AE10" s="8">
         <v>12636</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF10" s="8">
+        <v>13378</v>
+      </c>
+      <c r="AG10" s="32">
+        <v>14355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -4274,8 +4321,14 @@
       <c r="AE11" s="8">
         <v>4897</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF11" s="8">
+        <v>5539</v>
+      </c>
+      <c r="AG11" s="32">
+        <v>6238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -4369,8 +4422,14 @@
       <c r="AE12" s="8">
         <v>1976</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF12" s="8">
+        <v>2047</v>
+      </c>
+      <c r="AG12" s="32">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -4464,8 +4523,14 @@
       <c r="AE13" s="8">
         <v>3402</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF13" s="8">
+        <v>3707</v>
+      </c>
+      <c r="AG13" s="32">
+        <v>4165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4559,8 +4624,14 @@
       <c r="AE14" s="8">
         <v>7385</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF14" s="8">
+        <v>7806</v>
+      </c>
+      <c r="AG14" s="32">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -4654,8 +4725,14 @@
       <c r="AE15" s="8">
         <v>5422</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF15" s="8">
+        <v>5583</v>
+      </c>
+      <c r="AG15" s="32">
+        <v>6501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -4749,8 +4826,14 @@
       <c r="AE16" s="8">
         <v>5549</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF16" s="8">
+        <v>6090</v>
+      </c>
+      <c r="AG16" s="32">
+        <v>6640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -4843,6 +4926,12 @@
       </c>
       <c r="AE17" s="4">
         <v>42990</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>45968</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>50756</v>
       </c>
     </row>
   </sheetData>
@@ -4855,7 +4944,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE160"/>
+  <dimension ref="A1:AG160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
@@ -4873,42 +4962,42 @@
     <col min="25" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.7109375" customWidth="1"/>
     <col min="29" max="30" width="10.7109375" style="21" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B6" s="11"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -4933,7 +5022,7 @@
       <c r="AA7" s="21"/>
       <c r="AB7" s="21"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -5027,8 +5116,14 @@
       <c r="AE8" s="3">
         <v>43927</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF8" s="3">
+        <v>43928</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>43929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -5122,8 +5217,14 @@
       <c r="AE9" s="6">
         <v>1723</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF9" s="6">
+        <v>1818</v>
+      </c>
+      <c r="AG9" s="6">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>286</v>
       </c>
@@ -5217,8 +5318,14 @@
       <c r="AE10" s="8">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF10" s="8">
+        <v>36</v>
+      </c>
+      <c r="AG10" s="32">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>316</v>
       </c>
@@ -5312,8 +5419,14 @@
       <c r="AE11" s="8">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF11" s="8">
+        <v>169</v>
+      </c>
+      <c r="AG11" s="32">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>312</v>
       </c>
@@ -5407,8 +5520,14 @@
       <c r="AE12" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF12" s="8">
+        <v>112</v>
+      </c>
+      <c r="AG12" s="32">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>186</v>
       </c>
@@ -5502,8 +5621,14 @@
       <c r="AE13" s="8">
         <v>117</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF13" s="8">
+        <v>123</v>
+      </c>
+      <c r="AG13" s="32">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>290</v>
       </c>
@@ -5597,8 +5722,14 @@
       <c r="AE14" s="8">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF14" s="8">
+        <v>55</v>
+      </c>
+      <c r="AG14" s="32">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>254</v>
       </c>
@@ -5692,8 +5823,14 @@
       <c r="AE15" s="8">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF15" s="8">
+        <v>107</v>
+      </c>
+      <c r="AG15" s="32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>258</v>
       </c>
@@ -5787,8 +5924,14 @@
       <c r="AE16" s="8">
         <v>138</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF16" s="8">
+        <v>162</v>
+      </c>
+      <c r="AG16" s="32">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>304</v>
       </c>
@@ -5882,8 +6025,14 @@
       <c r="AE17" s="8">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF17" s="8">
+        <v>86</v>
+      </c>
+      <c r="AG17" s="32">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>282</v>
       </c>
@@ -5977,8 +6126,14 @@
       <c r="AE18" s="8">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF18" s="8">
+        <v>85</v>
+      </c>
+      <c r="AG18" s="32">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>308</v>
       </c>
@@ -6072,8 +6227,14 @@
       <c r="AE19" s="8">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF19" s="8">
+        <v>38</v>
+      </c>
+      <c r="AG19" s="32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>180</v>
       </c>
@@ -6167,8 +6328,14 @@
       <c r="AE20" s="8">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF20" s="8">
+        <v>97</v>
+      </c>
+      <c r="AG20" s="32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>318</v>
       </c>
@@ -6262,8 +6429,14 @@
       <c r="AE21" s="8">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF21" s="8">
+        <v>49</v>
+      </c>
+      <c r="AG21" s="32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>310</v>
       </c>
@@ -6357,8 +6530,14 @@
       <c r="AE22" s="8">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF22" s="8">
+        <v>62</v>
+      </c>
+      <c r="AG22" s="32">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>244</v>
       </c>
@@ -6452,8 +6631,14 @@
       <c r="AE23" s="8">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF23" s="8">
+        <v>75</v>
+      </c>
+      <c r="AG23" s="32">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>196</v>
       </c>
@@ -6547,8 +6732,14 @@
       <c r="AE24" s="8">
         <v>263</v>
       </c>
-    </row>
-    <row r="25" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF24" s="8">
+        <v>263</v>
+      </c>
+      <c r="AG24" s="32">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>238</v>
       </c>
@@ -6642,8 +6833,14 @@
       <c r="AE25" s="8">
         <v>211</v>
       </c>
-    </row>
-    <row r="26" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF25" s="8">
+        <v>211</v>
+      </c>
+      <c r="AG25" s="32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>320</v>
       </c>
@@ -6737,8 +6934,14 @@
       <c r="AE26" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF26" s="8">
+        <v>6</v>
+      </c>
+      <c r="AG26" s="32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>144</v>
       </c>
@@ -6832,8 +7035,14 @@
       <c r="AE27" s="8">
         <v>204</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF27" s="8">
+        <v>204</v>
+      </c>
+      <c r="AG27" s="32">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>274</v>
       </c>
@@ -6927,8 +7136,14 @@
       <c r="AE28" s="8">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF28" s="8">
+        <v>70</v>
+      </c>
+      <c r="AG28" s="32">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>322</v>
       </c>
@@ -7022,8 +7237,14 @@
       <c r="AE29" s="8">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF29" s="8">
+        <v>79</v>
+      </c>
+      <c r="AG29" s="32">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>288</v>
       </c>
@@ -7117,8 +7338,14 @@
       <c r="AE30" s="8">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF30" s="8">
+        <v>117</v>
+      </c>
+      <c r="AG30" s="32">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>246</v>
       </c>
@@ -7212,8 +7439,14 @@
       <c r="AE31" s="8">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF31" s="8">
+        <v>67</v>
+      </c>
+      <c r="AG31" s="32">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>166</v>
       </c>
@@ -7307,8 +7540,14 @@
       <c r="AE32" s="8">
         <v>211</v>
       </c>
-    </row>
-    <row r="33" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF32" s="8">
+        <v>211</v>
+      </c>
+      <c r="AG32" s="32">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>256</v>
       </c>
@@ -7402,8 +7641,14 @@
       <c r="AE33" s="8">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF33" s="8">
+        <v>82</v>
+      </c>
+      <c r="AG33" s="32">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>160</v>
       </c>
@@ -7497,8 +7742,14 @@
       <c r="AE34" s="8">
         <v>139</v>
       </c>
-    </row>
-    <row r="35" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF34" s="8">
+        <v>139</v>
+      </c>
+      <c r="AG34" s="32">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>216</v>
       </c>
@@ -7592,8 +7843,14 @@
       <c r="AE35" s="8">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF35" s="8">
+        <v>102</v>
+      </c>
+      <c r="AG35" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>202</v>
       </c>
@@ -7687,8 +7944,14 @@
       <c r="AE36" s="8">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF36" s="8">
+        <v>57</v>
+      </c>
+      <c r="AG36" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>250</v>
       </c>
@@ -7782,8 +8045,14 @@
       <c r="AE37" s="8">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF37" s="8">
+        <v>75</v>
+      </c>
+      <c r="AG37" s="32">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>294</v>
       </c>
@@ -7877,8 +8146,14 @@
       <c r="AE38" s="8">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF38" s="8">
+        <v>62</v>
+      </c>
+      <c r="AG38" s="32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>276</v>
       </c>
@@ -7972,8 +8247,14 @@
       <c r="AE39" s="8">
         <v>167</v>
       </c>
-    </row>
-    <row r="40" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF39" s="8">
+        <v>195</v>
+      </c>
+      <c r="AG39" s="32">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>262</v>
       </c>
@@ -8067,8 +8348,14 @@
       <c r="AE40" s="8">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF40" s="8">
+        <v>136</v>
+      </c>
+      <c r="AG40" s="32">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>268</v>
       </c>
@@ -8162,8 +8449,14 @@
       <c r="AE41" s="8">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF41" s="8">
+        <v>125</v>
+      </c>
+      <c r="AG41" s="32">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>198</v>
       </c>
@@ -8257,8 +8550,14 @@
       <c r="AE42" s="8">
         <v>153</v>
       </c>
-    </row>
-    <row r="43" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF42" s="8">
+        <v>196</v>
+      </c>
+      <c r="AG42" s="32">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>270</v>
       </c>
@@ -8352,8 +8651,14 @@
       <c r="AE43" s="8">
         <v>69</v>
       </c>
-    </row>
-    <row r="44" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF43" s="8">
+        <v>79</v>
+      </c>
+      <c r="AG43" s="32">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>280</v>
       </c>
@@ -8447,8 +8752,14 @@
       <c r="AE44" s="8">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF44" s="8">
+        <v>107</v>
+      </c>
+      <c r="AG44" s="32">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>218</v>
       </c>
@@ -8542,8 +8853,14 @@
       <c r="AE45" s="8">
         <v>111</v>
       </c>
-    </row>
-    <row r="46" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF45" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG45" s="32">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>116</v>
       </c>
@@ -8637,8 +8954,14 @@
       <c r="AE46" s="8">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF46" s="8">
+        <v>167</v>
+      </c>
+      <c r="AG46" s="32">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>150</v>
       </c>
@@ -8732,8 +9055,14 @@
       <c r="AE47" s="8">
         <v>105</v>
       </c>
-    </row>
-    <row r="48" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF47" s="8">
+        <v>116</v>
+      </c>
+      <c r="AG47" s="32">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>194</v>
       </c>
@@ -8827,8 +9156,14 @@
       <c r="AE48" s="8">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF48" s="8">
+        <v>129</v>
+      </c>
+      <c r="AG48" s="32">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>240</v>
       </c>
@@ -8922,8 +9257,14 @@
       <c r="AE49" s="8">
         <v>181</v>
       </c>
-    </row>
-    <row r="50" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF49" s="8">
+        <v>186</v>
+      </c>
+      <c r="AG49" s="32">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>164</v>
       </c>
@@ -9017,8 +9358,14 @@
       <c r="AE50" s="8">
         <v>85</v>
       </c>
-    </row>
-    <row r="51" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF50" s="8">
+        <v>86</v>
+      </c>
+      <c r="AG50" s="32">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>242</v>
       </c>
@@ -9112,8 +9459,14 @@
       <c r="AE51" s="8">
         <v>104</v>
       </c>
-    </row>
-    <row r="52" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF51" s="8">
+        <v>115</v>
+      </c>
+      <c r="AG51" s="32">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>210</v>
       </c>
@@ -9207,8 +9560,14 @@
       <c r="AE52" s="8">
         <v>149</v>
       </c>
-    </row>
-    <row r="53" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF52" s="8">
+        <v>181</v>
+      </c>
+      <c r="AG52" s="32">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>292</v>
       </c>
@@ -9302,8 +9661,14 @@
       <c r="AE53" s="8">
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF53" s="8">
+        <v>36</v>
+      </c>
+      <c r="AG53" s="32">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>236</v>
       </c>
@@ -9397,8 +9762,14 @@
       <c r="AE54" s="8">
         <v>292</v>
       </c>
-    </row>
-    <row r="55" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF54" s="8">
+        <v>303</v>
+      </c>
+      <c r="AG54" s="32">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>192</v>
       </c>
@@ -9492,8 +9863,14 @@
       <c r="AE55" s="8">
         <v>196</v>
       </c>
-    </row>
-    <row r="56" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF55" s="8">
+        <v>209</v>
+      </c>
+      <c r="AG55" s="32">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>212</v>
       </c>
@@ -9587,8 +9964,14 @@
       <c r="AE56" s="8">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF56" s="8">
+        <v>227</v>
+      </c>
+      <c r="AG56" s="32">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>278</v>
       </c>
@@ -9682,8 +10065,14 @@
       <c r="AE57" s="8">
         <v>143</v>
       </c>
-    </row>
-    <row r="58" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF57" s="8">
+        <v>157</v>
+      </c>
+      <c r="AG57" s="32">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>178</v>
       </c>
@@ -9777,8 +10166,14 @@
       <c r="AE58" s="8">
         <v>198</v>
       </c>
-    </row>
-    <row r="59" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF58" s="8">
+        <v>198</v>
+      </c>
+      <c r="AG58" s="32">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>162</v>
       </c>
@@ -9872,8 +10267,14 @@
       <c r="AE59" s="8">
         <v>154</v>
       </c>
-    </row>
-    <row r="60" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF59" s="8">
+        <v>156</v>
+      </c>
+      <c r="AG59" s="32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>302</v>
       </c>
@@ -9967,8 +10368,14 @@
       <c r="AE60" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="61" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF60" s="8">
+        <v>120</v>
+      </c>
+      <c r="AG60" s="32">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>222</v>
       </c>
@@ -10062,8 +10469,14 @@
       <c r="AE61" s="8">
         <v>144</v>
       </c>
-    </row>
-    <row r="62" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF61" s="8">
+        <v>164</v>
+      </c>
+      <c r="AG61" s="32">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>230</v>
       </c>
@@ -10157,8 +10570,14 @@
       <c r="AE62" s="8">
         <v>211</v>
       </c>
-    </row>
-    <row r="63" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF62" s="8">
+        <v>211</v>
+      </c>
+      <c r="AG62" s="32">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>190</v>
       </c>
@@ -10252,8 +10671,14 @@
       <c r="AE63" s="8">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF63" s="8">
+        <v>116</v>
+      </c>
+      <c r="AG63" s="32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>214</v>
       </c>
@@ -10347,8 +10772,14 @@
       <c r="AE64" s="8">
         <v>126</v>
       </c>
-    </row>
-    <row r="65" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF64" s="8">
+        <v>126</v>
+      </c>
+      <c r="AG64" s="32">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>188</v>
       </c>
@@ -10442,8 +10873,14 @@
       <c r="AE65" s="8">
         <v>170</v>
       </c>
-    </row>
-    <row r="66" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF65" s="8">
+        <v>185</v>
+      </c>
+      <c r="AG65" s="32">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>204</v>
       </c>
@@ -10537,8 +10974,14 @@
       <c r="AE66" s="8">
         <v>138</v>
       </c>
-    </row>
-    <row r="67" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF66" s="8">
+        <v>151</v>
+      </c>
+      <c r="AG66" s="32">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>106</v>
       </c>
@@ -10632,8 +11075,14 @@
       <c r="AE67" s="8">
         <v>323</v>
       </c>
-    </row>
-    <row r="68" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF67" s="8">
+        <v>361</v>
+      </c>
+      <c r="AG67" s="32">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="68" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>138</v>
       </c>
@@ -10727,8 +11176,14 @@
       <c r="AE68" s="8">
         <v>216</v>
       </c>
-    </row>
-    <row r="69" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF68" s="8">
+        <v>232</v>
+      </c>
+      <c r="AG68" s="32">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>184</v>
       </c>
@@ -10822,8 +11277,14 @@
       <c r="AE69" s="8">
         <v>167</v>
       </c>
-    </row>
-    <row r="70" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF69" s="8">
+        <v>186</v>
+      </c>
+      <c r="AG69" s="32">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>182</v>
       </c>
@@ -10917,8 +11378,14 @@
       <c r="AE70" s="8">
         <v>242</v>
       </c>
-    </row>
-    <row r="71" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF70" s="8">
+        <v>259</v>
+      </c>
+      <c r="AG70" s="32">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>146</v>
       </c>
@@ -11012,8 +11479,14 @@
       <c r="AE71" s="8">
         <v>246</v>
       </c>
-    </row>
-    <row r="72" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF71" s="8">
+        <v>270</v>
+      </c>
+      <c r="AG71" s="32">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>142</v>
       </c>
@@ -11107,8 +11580,14 @@
       <c r="AE72" s="8">
         <v>162</v>
       </c>
-    </row>
-    <row r="73" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF72" s="8">
+        <v>182</v>
+      </c>
+      <c r="AG72" s="32">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>156</v>
       </c>
@@ -11202,8 +11681,14 @@
       <c r="AE73" s="8">
         <v>222</v>
       </c>
-    </row>
-    <row r="74" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF73" s="8">
+        <v>240</v>
+      </c>
+      <c r="AG73" s="32">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="74" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>260</v>
       </c>
@@ -11297,8 +11782,14 @@
       <c r="AE74" s="8">
         <v>185</v>
       </c>
-    </row>
-    <row r="75" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF74" s="8">
+        <v>197</v>
+      </c>
+      <c r="AG74" s="32">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="75" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>264</v>
       </c>
@@ -11392,8 +11883,14 @@
       <c r="AE75" s="8">
         <v>167</v>
       </c>
-    </row>
-    <row r="76" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF75" s="8">
+        <v>169</v>
+      </c>
+      <c r="AG75" s="32">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>154</v>
       </c>
@@ -11487,8 +11984,14 @@
       <c r="AE76" s="8">
         <v>510</v>
       </c>
-    </row>
-    <row r="77" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF76" s="8">
+        <v>552</v>
+      </c>
+      <c r="AG76" s="32">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="77" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>298</v>
       </c>
@@ -11582,8 +12085,14 @@
       <c r="AE77" s="8">
         <v>236</v>
       </c>
-    </row>
-    <row r="78" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF77" s="8">
+        <v>239</v>
+      </c>
+      <c r="AG77" s="32">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>232</v>
       </c>
@@ -11677,8 +12186,14 @@
       <c r="AE78" s="8">
         <v>264</v>
       </c>
-    </row>
-    <row r="79" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF78" s="8">
+        <v>289</v>
+      </c>
+      <c r="AG78" s="32">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>208</v>
       </c>
@@ -11772,8 +12287,14 @@
       <c r="AE79" s="8">
         <v>220</v>
       </c>
-    </row>
-    <row r="80" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF79" s="8">
+        <v>262</v>
+      </c>
+      <c r="AG79" s="32">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="80" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>220</v>
       </c>
@@ -11867,8 +12388,14 @@
       <c r="AE80" s="8">
         <v>216</v>
       </c>
-    </row>
-    <row r="81" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF80" s="8">
+        <v>216</v>
+      </c>
+      <c r="AG80" s="32">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>300</v>
       </c>
@@ -11962,8 +12489,14 @@
       <c r="AE81" s="8">
         <v>144</v>
       </c>
-    </row>
-    <row r="82" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF81" s="8">
+        <v>144</v>
+      </c>
+      <c r="AG81" s="32">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>284</v>
       </c>
@@ -12057,8 +12590,14 @@
       <c r="AE82" s="8">
         <v>221</v>
       </c>
-    </row>
-    <row r="83" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF82" s="8">
+        <v>223</v>
+      </c>
+      <c r="AG82" s="32">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="83" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>54</v>
       </c>
@@ -12152,8 +12691,14 @@
       <c r="AE83" s="8">
         <v>882</v>
       </c>
-    </row>
-    <row r="84" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF83" s="8">
+        <v>883</v>
+      </c>
+      <c r="AG83" s="32">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="84" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>108</v>
       </c>
@@ -12247,8 +12792,14 @@
       <c r="AE84" s="8">
         <v>359</v>
       </c>
-    </row>
-    <row r="85" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF84" s="8">
+        <v>367</v>
+      </c>
+      <c r="AG84" s="32">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="85" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>174</v>
       </c>
@@ -12342,8 +12893,14 @@
       <c r="AE85" s="8">
         <v>180</v>
       </c>
-    </row>
-    <row r="86" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF85" s="8">
+        <v>183</v>
+      </c>
+      <c r="AG85" s="32">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>296</v>
       </c>
@@ -12437,8 +12994,14 @@
       <c r="AE86" s="8">
         <v>98</v>
       </c>
-    </row>
-    <row r="87" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF86" s="8">
+        <v>101</v>
+      </c>
+      <c r="AG86" s="32">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>248</v>
       </c>
@@ -12532,8 +13095,14 @@
       <c r="AE87" s="8">
         <v>278</v>
       </c>
-    </row>
-    <row r="88" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF87" s="8">
+        <v>285</v>
+      </c>
+      <c r="AG87" s="32">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="88" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>68</v>
       </c>
@@ -12627,8 +13196,14 @@
       <c r="AE88" s="8">
         <v>1287</v>
       </c>
-    </row>
-    <row r="89" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF88" s="8">
+        <v>1372</v>
+      </c>
+      <c r="AG88" s="32">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="89" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>252</v>
       </c>
@@ -12722,8 +13297,14 @@
       <c r="AE89" s="8">
         <v>263</v>
       </c>
-    </row>
-    <row r="90" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF89" s="8">
+        <v>277</v>
+      </c>
+      <c r="AG89" s="32">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="90" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>170</v>
       </c>
@@ -12817,8 +13398,14 @@
       <c r="AE90" s="8">
         <v>296</v>
       </c>
-    </row>
-    <row r="91" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF90" s="8">
+        <v>309</v>
+      </c>
+      <c r="AG90" s="32">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>224</v>
       </c>
@@ -12912,8 +13499,14 @@
       <c r="AE91" s="8">
         <v>353</v>
       </c>
-    </row>
-    <row r="92" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF91" s="8">
+        <v>363</v>
+      </c>
+      <c r="AG91" s="32">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="92" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>314</v>
       </c>
@@ -13007,8 +13600,14 @@
       <c r="AE92" s="8">
         <v>215</v>
       </c>
-    </row>
-    <row r="93" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF92" s="8">
+        <v>241</v>
+      </c>
+      <c r="AG92" s="32">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="93" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>124</v>
       </c>
@@ -13102,8 +13701,14 @@
       <c r="AE93" s="8">
         <v>359</v>
       </c>
-    </row>
-    <row r="94" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF93" s="8">
+        <v>386</v>
+      </c>
+      <c r="AG93" s="32">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="94" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>92</v>
       </c>
@@ -13197,8 +13802,14 @@
       <c r="AE94" s="8">
         <v>304</v>
       </c>
-    </row>
-    <row r="95" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF94" s="8">
+        <v>335</v>
+      </c>
+      <c r="AG94" s="32">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="95" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>228</v>
       </c>
@@ -13292,8 +13903,14 @@
       <c r="AE95" s="8">
         <v>204</v>
       </c>
-    </row>
-    <row r="96" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF95" s="8">
+        <v>222</v>
+      </c>
+      <c r="AG95" s="32">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="96" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>272</v>
       </c>
@@ -13387,8 +14004,14 @@
       <c r="AE96" s="8">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF96" s="8">
+        <v>94</v>
+      </c>
+      <c r="AG96" s="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>266</v>
       </c>
@@ -13482,8 +14105,14 @@
       <c r="AE97" s="8">
         <v>198</v>
       </c>
-    </row>
-    <row r="98" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF97" s="8">
+        <v>203</v>
+      </c>
+      <c r="AG97" s="32">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>130</v>
       </c>
@@ -13577,8 +14206,14 @@
       <c r="AE98" s="8">
         <v>325</v>
       </c>
-    </row>
-    <row r="99" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF98" s="8">
+        <v>340</v>
+      </c>
+      <c r="AG98" s="32">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="99" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>234</v>
       </c>
@@ -13672,8 +14307,14 @@
       <c r="AE99" s="8">
         <v>162</v>
       </c>
-    </row>
-    <row r="100" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF99" s="8">
+        <v>177</v>
+      </c>
+      <c r="AG99" s="32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>306</v>
       </c>
@@ -13767,8 +14408,14 @@
       <c r="AE100" s="8">
         <v>180</v>
       </c>
-    </row>
-    <row r="101" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF100" s="8">
+        <v>188</v>
+      </c>
+      <c r="AG100" s="32">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>112</v>
       </c>
@@ -13862,8 +14509,14 @@
       <c r="AE101" s="8">
         <v>211</v>
       </c>
-    </row>
-    <row r="102" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF101" s="8">
+        <v>222</v>
+      </c>
+      <c r="AG101" s="32">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>96</v>
       </c>
@@ -13957,8 +14610,14 @@
       <c r="AE102" s="8">
         <v>666</v>
       </c>
-    </row>
-    <row r="103" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF102" s="8">
+        <v>717</v>
+      </c>
+      <c r="AG102" s="32">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="103" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>104</v>
       </c>
@@ -14052,8 +14711,14 @@
       <c r="AE103" s="8">
         <v>250</v>
       </c>
-    </row>
-    <row r="104" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF103" s="8">
+        <v>274</v>
+      </c>
+      <c r="AG103" s="32">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="104" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>36</v>
       </c>
@@ -14147,8 +14812,14 @@
       <c r="AE104" s="8">
         <v>759</v>
       </c>
-    </row>
-    <row r="105" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF104" s="8">
+        <v>819</v>
+      </c>
+      <c r="AG104" s="32">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="105" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>52</v>
       </c>
@@ -14242,8 +14913,14 @@
       <c r="AE105" s="8">
         <v>521</v>
       </c>
-    </row>
-    <row r="106" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF105" s="8">
+        <v>547</v>
+      </c>
+      <c r="AG105" s="32">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="106" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>64</v>
       </c>
@@ -14337,8 +15014,14 @@
       <c r="AE106" s="8">
         <v>298</v>
       </c>
-    </row>
-    <row r="107" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF106" s="8">
+        <v>321</v>
+      </c>
+      <c r="AG106" s="32">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="107" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>46</v>
       </c>
@@ -14432,8 +15115,14 @@
       <c r="AE107" s="8">
         <v>620</v>
       </c>
-    </row>
-    <row r="108" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF107" s="8">
+        <v>689</v>
+      </c>
+      <c r="AG107" s="32">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="108" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>42</v>
       </c>
@@ -14527,8 +15216,14 @@
       <c r="AE108" s="8">
         <v>503</v>
       </c>
-    </row>
-    <row r="109" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF108" s="8">
+        <v>533</v>
+      </c>
+      <c r="AG108" s="32">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="109" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>84</v>
       </c>
@@ -14622,8 +15317,14 @@
       <c r="AE109" s="8">
         <v>350</v>
       </c>
-    </row>
-    <row r="110" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF109" s="8">
+        <v>370</v>
+      </c>
+      <c r="AG109" s="32">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="110" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>72</v>
       </c>
@@ -14717,8 +15418,14 @@
       <c r="AE110" s="8">
         <v>322</v>
       </c>
-    </row>
-    <row r="111" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF110" s="8">
+        <v>337</v>
+      </c>
+      <c r="AG110" s="32">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="111" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>78</v>
       </c>
@@ -14812,8 +15519,14 @@
       <c r="AE111" s="8">
         <v>362</v>
       </c>
-    </row>
-    <row r="112" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF111" s="8">
+        <v>365</v>
+      </c>
+      <c r="AG111" s="32">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="112" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>94</v>
       </c>
@@ -14907,8 +15620,14 @@
       <c r="AE112" s="8">
         <v>266</v>
       </c>
-    </row>
-    <row r="113" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF112" s="8">
+        <v>286</v>
+      </c>
+      <c r="AG112" s="32">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="113" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>80</v>
       </c>
@@ -15002,8 +15721,14 @@
       <c r="AE113" s="8">
         <v>285</v>
       </c>
-    </row>
-    <row r="114" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF113" s="8">
+        <v>308</v>
+      </c>
+      <c r="AG113" s="32">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="114" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>40</v>
       </c>
@@ -15097,8 +15822,14 @@
       <c r="AE114" s="8">
         <v>469</v>
       </c>
-    </row>
-    <row r="115" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF114" s="8">
+        <v>500</v>
+      </c>
+      <c r="AG114" s="32">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="115" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>134</v>
       </c>
@@ -15192,8 +15923,14 @@
       <c r="AE115" s="8">
         <v>248</v>
       </c>
-    </row>
-    <row r="116" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF115" s="8">
+        <v>273</v>
+      </c>
+      <c r="AG115" s="32">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="116" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>86</v>
       </c>
@@ -15287,8 +16024,14 @@
       <c r="AE116" s="8">
         <v>348</v>
       </c>
-    </row>
-    <row r="117" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF116" s="8">
+        <v>366</v>
+      </c>
+      <c r="AG116" s="32">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="117" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>88</v>
       </c>
@@ -15382,8 +16125,14 @@
       <c r="AE117" s="8">
         <v>338</v>
       </c>
-    </row>
-    <row r="118" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF117" s="8">
+        <v>361</v>
+      </c>
+      <c r="AG117" s="32">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="118" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>66</v>
       </c>
@@ -15477,8 +16226,14 @@
       <c r="AE118" s="8">
         <v>257</v>
       </c>
-    </row>
-    <row r="119" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF118" s="8">
+        <v>268</v>
+      </c>
+      <c r="AG118" s="32">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="119" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>38</v>
       </c>
@@ -15572,8 +16327,14 @@
       <c r="AE119" s="8">
         <v>272</v>
       </c>
-    </row>
-    <row r="120" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF119" s="8">
+        <v>278</v>
+      </c>
+      <c r="AG119" s="32">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="120" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>136</v>
       </c>
@@ -15667,8 +16428,14 @@
       <c r="AE120" s="8">
         <v>169</v>
       </c>
-    </row>
-    <row r="121" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF120" s="8">
+        <v>199</v>
+      </c>
+      <c r="AG120" s="32">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="121" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>30</v>
       </c>
@@ -15762,8 +16529,14 @@
       <c r="AE121" s="8">
         <v>671</v>
       </c>
-    </row>
-    <row r="122" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF121" s="8">
+        <v>698</v>
+      </c>
+      <c r="AG121" s="32">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="122" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>56</v>
       </c>
@@ -15857,8 +16630,14 @@
       <c r="AE122" s="8">
         <v>490</v>
       </c>
-    </row>
-    <row r="123" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF122" s="8">
+        <v>516</v>
+      </c>
+      <c r="AG122" s="32">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="123" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>60</v>
       </c>
@@ -15952,8 +16731,14 @@
       <c r="AE123" s="8">
         <v>316</v>
       </c>
-    </row>
-    <row r="124" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF123" s="8">
+        <v>358</v>
+      </c>
+      <c r="AG123" s="32">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>76</v>
       </c>
@@ -16047,8 +16832,14 @@
       <c r="AE124" s="8">
         <v>530</v>
       </c>
-    </row>
-    <row r="125" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF124" s="8">
+        <v>535</v>
+      </c>
+      <c r="AG124" s="32">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="125" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>110</v>
       </c>
@@ -16142,8 +16933,14 @@
       <c r="AE125" s="8">
         <v>311</v>
       </c>
-    </row>
-    <row r="126" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF125" s="8">
+        <v>319</v>
+      </c>
+      <c r="AG125" s="32">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="126" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>158</v>
       </c>
@@ -16237,8 +17034,14 @@
       <c r="AE126" s="8">
         <v>200</v>
       </c>
-    </row>
-    <row r="127" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF126" s="8">
+        <v>213</v>
+      </c>
+      <c r="AG126" s="32">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="127" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>28</v>
       </c>
@@ -16332,8 +17135,14 @@
       <c r="AE127" s="8">
         <v>685</v>
       </c>
-    </row>
-    <row r="128" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF127" s="8">
+        <v>710</v>
+      </c>
+      <c r="AG127" s="32">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="128" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>140</v>
       </c>
@@ -16427,8 +17236,14 @@
       <c r="AE128" s="8">
         <v>262</v>
       </c>
-    </row>
-    <row r="129" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF128" s="8">
+        <v>287</v>
+      </c>
+      <c r="AG128" s="32">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>74</v>
       </c>
@@ -16522,8 +17337,14 @@
       <c r="AE129" s="8">
         <v>359</v>
       </c>
-    </row>
-    <row r="130" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF129" s="8">
+        <v>361</v>
+      </c>
+      <c r="AG129" s="32">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="130" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>120</v>
       </c>
@@ -16617,8 +17438,14 @@
       <c r="AE130" s="8">
         <v>389</v>
       </c>
-    </row>
-    <row r="131" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF130" s="8">
+        <v>393</v>
+      </c>
+      <c r="AG130" s="32">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="131" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>34</v>
       </c>
@@ -16712,8 +17539,14 @@
       <c r="AE131" s="8">
         <v>526</v>
       </c>
-    </row>
-    <row r="132" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF131" s="8">
+        <v>557</v>
+      </c>
+      <c r="AG131" s="32">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="132" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -16807,8 +17640,14 @@
       <c r="AE132" s="8">
         <v>383</v>
       </c>
-    </row>
-    <row r="133" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF132" s="8">
+        <v>398</v>
+      </c>
+      <c r="AG132" s="32">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="133" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>58</v>
       </c>
@@ -16902,8 +17741,14 @@
       <c r="AE133" s="8">
         <v>300</v>
       </c>
-    </row>
-    <row r="134" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF133" s="8">
+        <v>329</v>
+      </c>
+      <c r="AG133" s="32">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="134" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>132</v>
       </c>
@@ -16997,8 +17842,14 @@
       <c r="AE134" s="8">
         <v>222</v>
       </c>
-    </row>
-    <row r="135" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF134" s="8">
+        <v>237</v>
+      </c>
+      <c r="AG134" s="32">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="135" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>62</v>
       </c>
@@ -17092,8 +17943,14 @@
       <c r="AE135" s="8">
         <v>753</v>
       </c>
-    </row>
-    <row r="136" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF135" s="8">
+        <v>804</v>
+      </c>
+      <c r="AG135" s="32">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="136" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>50</v>
       </c>
@@ -17187,8 +18044,14 @@
       <c r="AE136" s="8">
         <v>494</v>
       </c>
-    </row>
-    <row r="137" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF136" s="8">
+        <v>501</v>
+      </c>
+      <c r="AG136" s="32">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="137" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>98</v>
       </c>
@@ -17282,8 +18145,14 @@
       <c r="AE137" s="8">
         <v>229</v>
       </c>
-    </row>
-    <row r="138" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF137" s="8">
+        <v>236</v>
+      </c>
+      <c r="AG137" s="32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="138" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>206</v>
       </c>
@@ -17377,8 +18246,14 @@
       <c r="AE138" s="8">
         <v>161</v>
       </c>
-    </row>
-    <row r="139" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF138" s="8">
+        <v>181</v>
+      </c>
+      <c r="AG138" s="32">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="139" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>82</v>
       </c>
@@ -17472,8 +18347,14 @@
       <c r="AE139" s="8">
         <v>858</v>
       </c>
-    </row>
-    <row r="140" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF139" s="8">
+        <v>938</v>
+      </c>
+      <c r="AG139" s="32">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="140" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>128</v>
       </c>
@@ -17567,8 +18448,14 @@
       <c r="AE140" s="8">
         <v>306</v>
       </c>
-    </row>
-    <row r="141" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF140" s="8">
+        <v>364</v>
+      </c>
+      <c r="AG140" s="32">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="141" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>26</v>
       </c>
@@ -17662,8 +18549,14 @@
       <c r="AE141" s="8">
         <v>921</v>
       </c>
-    </row>
-    <row r="142" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF141" s="8">
+        <v>989</v>
+      </c>
+      <c r="AG141" s="32">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="142" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>44</v>
       </c>
@@ -17757,8 +18650,14 @@
       <c r="AE142" s="8">
         <v>870</v>
       </c>
-    </row>
-    <row r="143" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF142" s="8">
+        <v>933</v>
+      </c>
+      <c r="AG142" s="32">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="143" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>100</v>
       </c>
@@ -17852,8 +18751,14 @@
       <c r="AE143" s="8">
         <v>791</v>
       </c>
-    </row>
-    <row r="144" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF143" s="8">
+        <v>923</v>
+      </c>
+      <c r="AG143" s="32">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="144" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>102</v>
       </c>
@@ -17947,8 +18852,14 @@
       <c r="AE144" s="8">
         <v>838</v>
       </c>
-    </row>
-    <row r="145" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF144" s="8">
+        <v>923</v>
+      </c>
+      <c r="AG144" s="32">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="145" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>118</v>
       </c>
@@ -18042,8 +18953,14 @@
       <c r="AE145" s="8">
         <v>338</v>
       </c>
-    </row>
-    <row r="146" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF145" s="8">
+        <v>339</v>
+      </c>
+      <c r="AG145" s="32">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="146" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>226</v>
       </c>
@@ -18137,8 +19054,14 @@
       <c r="AE146" s="8">
         <v>275</v>
       </c>
-    </row>
-    <row r="147" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF146" s="8">
+        <v>277</v>
+      </c>
+      <c r="AG146" s="32">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="147" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>168</v>
       </c>
@@ -18232,8 +19155,14 @@
       <c r="AE147" s="8">
         <v>301</v>
       </c>
-    </row>
-    <row r="148" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF147" s="8">
+        <v>341</v>
+      </c>
+      <c r="AG147" s="32">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="148" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>126</v>
       </c>
@@ -18327,8 +19256,14 @@
       <c r="AE148" s="8">
         <v>428</v>
       </c>
-    </row>
-    <row r="149" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF148" s="8">
+        <v>473</v>
+      </c>
+      <c r="AG148" s="32">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="149" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>152</v>
       </c>
@@ -18422,8 +19357,14 @@
       <c r="AE149" s="8">
         <v>269</v>
       </c>
-    </row>
-    <row r="150" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF149" s="8">
+        <v>285</v>
+      </c>
+      <c r="AG149" s="32">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="150" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>90</v>
       </c>
@@ -18517,8 +19458,14 @@
       <c r="AE150" s="8">
         <v>425</v>
       </c>
-    </row>
-    <row r="151" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF150" s="8">
+        <v>469</v>
+      </c>
+      <c r="AG150" s="32">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="151" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>70</v>
       </c>
@@ -18612,8 +19559,14 @@
       <c r="AE151" s="8">
         <v>450</v>
       </c>
-    </row>
-    <row r="152" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF151" s="8">
+        <v>501</v>
+      </c>
+      <c r="AG151" s="32">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="152" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>176</v>
       </c>
@@ -18707,8 +19660,14 @@
       <c r="AE152" s="8">
         <v>114</v>
       </c>
-    </row>
-    <row r="153" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF152" s="8">
+        <v>114</v>
+      </c>
+      <c r="AG152" s="32">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="153" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>114</v>
       </c>
@@ -18802,8 +19761,14 @@
       <c r="AE153" s="8">
         <v>570</v>
       </c>
-    </row>
-    <row r="154" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF153" s="8">
+        <v>597</v>
+      </c>
+      <c r="AG153" s="32">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="154" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>148</v>
       </c>
@@ -18897,8 +19862,14 @@
       <c r="AE154" s="8">
         <v>243</v>
       </c>
-    </row>
-    <row r="155" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF154" s="8">
+        <v>263</v>
+      </c>
+      <c r="AG154" s="32">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="155" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>48</v>
       </c>
@@ -18992,8 +19963,14 @@
       <c r="AE155" s="8">
         <v>887</v>
       </c>
-    </row>
-    <row r="156" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF155" s="8">
+        <v>1017</v>
+      </c>
+      <c r="AG155" s="32">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="156" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>172</v>
       </c>
@@ -19087,8 +20064,14 @@
       <c r="AE156" s="8">
         <v>361</v>
       </c>
-    </row>
-    <row r="157" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF156" s="8">
+        <v>400</v>
+      </c>
+      <c r="AG156" s="32">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="157" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>122</v>
       </c>
@@ -19182,8 +20165,14 @@
       <c r="AE157" s="8">
         <v>224</v>
       </c>
-    </row>
-    <row r="158" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AF157" s="8">
+        <v>266</v>
+      </c>
+      <c r="AG157" s="32">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="158" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>200</v>
       </c>
@@ -19277,8 +20266,14 @@
       <c r="AE158" s="8">
         <v>394</v>
       </c>
-    </row>
-    <row r="159" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF158" s="8">
+        <v>419</v>
+      </c>
+      <c r="AG158" s="32">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>0</v>
       </c>
@@ -19372,8 +20367,14 @@
       <c r="AE159" s="4">
         <v>42990</v>
       </c>
-    </row>
-    <row r="160" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF159" s="4">
+        <v>45968</v>
+      </c>
+      <c r="AG159" s="4">
+        <v>50756</v>
+      </c>
+    </row>
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="AB160" s="21"/>
     </row>
   </sheetData>

</xml_diff>